<commit_message>
Updated UI systems and fixed some bugs
</commit_message>
<xml_diff>
--- a/Design Docs/Tasks.xlsx
+++ b/Design Docs/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\SpellCaster-FPS-Thing\Design Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DBC28C-5F63-4FFD-B462-67052F8BFACC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AF575B-7DDC-422A-957A-B1A84EB02812}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>Task Name</t>
   </si>
@@ -90,20 +90,59 @@
     <t>Default Spell Names</t>
   </si>
   <si>
-    <t>NPC Hit awareness</t>
-  </si>
-  <si>
     <t>NPC Hit state/animation</t>
   </si>
   <si>
     <t>Suspended</t>
+  </si>
+  <si>
+    <t>Defer?</t>
+  </si>
+  <si>
+    <t>Redesign shooting system</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>Projectile physics fix</t>
+  </si>
+  <si>
+    <t>Projectiles have a tendency to clip past colliders. Need to resolve this somehow.</t>
+  </si>
+  <si>
+    <t>Magic projectiles are slow and are very hard to hit, especially without AoE. Perhaps raycast and rotate to target is a better choice?</t>
+  </si>
+  <si>
+    <t>NPC reactions upon getting damaged</t>
+  </si>
+  <si>
+    <t>Enemies need to react to receiving hits. Should attempt to find and engage assailant</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Fixed?</t>
+  </si>
+  <si>
+    <t>Limit number of characters that can be spawned with summon</t>
+  </si>
+  <si>
+    <t>Spell casters (especially players) need to have a hard limit to prevent performance issues/exploits. Could be tied to spell tier</t>
+  </si>
+  <si>
+    <t>If player does not enter spell name before crafting, a default name is automatically generated and assigned to the spell</t>
+  </si>
+  <si>
+    <t>Hitstun state for enemies that have received damage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,8 +159,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +193,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="6">
     <border>
@@ -218,22 +271,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,15 +570,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" style="1" customWidth="1"/>
     <col min="3" max="4" width="13.21875" style="2" customWidth="1"/>
     <col min="5" max="5" width="120" style="2" customWidth="1"/>
@@ -545,135 +601,192 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="9" t="s">
+      <c r="E3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="13">
+        <v>2</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="10">
+        <v>1</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C6" s="10">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="D6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="10">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="12" t="s">
+      <c r="D7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C8" s="10">
         <v>1</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="12" t="s">
+      <c r="E8" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C9" s="10">
         <v>1</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="E9" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C10" s="16">
         <v>2</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D10" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="16">
+        <v>2</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="10">
+        <v>1</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="13"/>
-    </row>
-    <row r="8" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="13">
-        <v>1</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="13"/>
-    </row>
-    <row r="9" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="13">
-        <v>1</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="13"/>
+      <c r="E12" s="10" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
NPC reaction to being damaged
</commit_message>
<xml_diff>
--- a/Design Docs/Tasks.xlsx
+++ b/Design Docs/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\SpellCaster-FPS-Thing\Design Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68AF575B-7DDC-422A-957A-B1A84EB02812}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66618BD9-DE83-48CA-B1A0-EE1A4322124E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
   <si>
     <t>Task Name</t>
   </si>
@@ -136,6 +136,60 @@
   </si>
   <si>
     <t>Hitstun state for enemies that have received damage</t>
+  </si>
+  <si>
+    <t>Create lateral animations for damage and movement</t>
+  </si>
+  <si>
+    <t>Polish to bronze tier animations for test humans</t>
+  </si>
+  <si>
+    <t>Integrate animations into Blend Trees in Animator</t>
+  </si>
+  <si>
+    <t>Knock back tiers</t>
+  </si>
+  <si>
+    <t>Have knockback/power meet certain thresholds before applying force to the character</t>
+  </si>
+  <si>
+    <t>Bronze tier art pass on magic projectile visuals</t>
+  </si>
+  <si>
+    <t>Magic projectiles look like ass. Fix this.</t>
+  </si>
+  <si>
+    <t>Fix UI inventory items &gt; 1 disappearing from view grid</t>
+  </si>
+  <si>
+    <t>Playtest this motherfucker!</t>
+  </si>
+  <si>
+    <t>Actually play arena mode</t>
+  </si>
+  <si>
+    <t>Handling transitioning from damaged state</t>
+  </si>
+  <si>
+    <t>Have AI states uniquely determine if/how to change state when character takes damage</t>
+  </si>
+  <si>
+    <t>UI Health bar</t>
+  </si>
+  <si>
+    <t>UI Mana bar</t>
+  </si>
+  <si>
+    <t>Highlighted spell slot</t>
+  </si>
+  <si>
+    <t>Searching for target animation(s)</t>
+  </si>
+  <si>
+    <t>Enemy Health Bar</t>
+  </si>
+  <si>
+    <t>Enemy World Space UI</t>
   </si>
 </sst>
 </file>
@@ -200,7 +254,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -267,29 +321,221 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,22 +816,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" style="7" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="13.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="120" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="99.6640625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -597,196 +844,414 @@
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="17">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="22">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="13">
-        <v>2</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="27">
+        <v>2</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="32">
         <v>1</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="D5" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="32">
         <v>1</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="10" t="s">
+      <c r="D6" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="37">
+        <v>2</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="32">
+        <v>1</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="10">
-        <v>2</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="C9" s="32">
+        <v>1</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="44" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="42">
+        <v>2</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="42">
+        <v>2</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="34" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C12" s="32">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="9" t="s">
+      <c r="D12" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="32">
+        <v>2</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="33"/>
+    </row>
+    <row r="14" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C14" s="32">
+        <v>2</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="33"/>
+    </row>
+    <row r="15" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="32">
+        <v>2</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="33"/>
+    </row>
+    <row r="16" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="52">
         <v>1</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="15" t="s">
+      <c r="D16" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="16">
-        <v>2</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="16">
-        <v>2</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="C17" s="47">
+        <v>2</v>
+      </c>
+      <c r="D17" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="52">
+        <v>1</v>
+      </c>
+      <c r="D18" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="53"/>
+    </row>
+    <row r="19" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C19" s="12">
         <v>1</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>34</v>
-      </c>
+      <c r="D19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="47">
+        <v>1</v>
+      </c>
+      <c r="D20" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="47">
+        <v>2</v>
+      </c>
+      <c r="D21" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="48"/>
+    </row>
+    <row r="22" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="47">
+        <v>2</v>
+      </c>
+      <c r="D22" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="48"/>
+    </row>
+    <row r="23" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="47">
+        <v>2</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="48"/>
+    </row>
+    <row r="24" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="47">
+        <v>2</v>
+      </c>
+      <c r="D24" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="48"/>
+    </row>
+    <row r="25" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="47">
+        <v>2</v>
+      </c>
+      <c r="D25" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="48"/>
+    </row>
+    <row r="26" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="47">
+        <v>2</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Building Tutorial Level Graybox
This is V2 of the tutorial level
</commit_message>
<xml_diff>
--- a/Design Docs/Tasks.xlsx
+++ b/Design Docs/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\SpellCaster-FPS-Thing\Design Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66618BD9-DE83-48CA-B1A0-EE1A4322124E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312AD015-C4B0-4EB1-918E-8F0872AD2050}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
   <si>
     <t>Task Name</t>
   </si>
@@ -174,15 +174,6 @@
     <t>Have AI states uniquely determine if/how to change state when character takes damage</t>
   </si>
   <si>
-    <t>UI Health bar</t>
-  </si>
-  <si>
-    <t>UI Mana bar</t>
-  </si>
-  <si>
-    <t>Highlighted spell slot</t>
-  </si>
-  <si>
     <t>Searching for target animation(s)</t>
   </si>
   <si>
@@ -190,6 +181,27 @@
   </si>
   <si>
     <t>Enemy World Space UI</t>
+  </si>
+  <si>
+    <t>UI Health bar MVP</t>
+  </si>
+  <si>
+    <t>UI Mana bar MVP</t>
+  </si>
+  <si>
+    <t>Highlighted spell slot MVP</t>
+  </si>
+  <si>
+    <t>Disable craft spell button if spell is not yet valid</t>
+  </si>
+  <si>
+    <t>Add fade in to intro cinematic</t>
+  </si>
+  <si>
+    <t>Investigate starting instantly from tutorial cinematic</t>
+  </si>
+  <si>
+    <t>Black screen in CrossScenePersisted Object</t>
   </si>
 </sst>
 </file>
@@ -816,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1165,10 +1177,10 @@
     </row>
     <row r="21" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="45" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="47">
         <v>2</v>
@@ -1180,10 +1192,10 @@
     </row>
     <row r="22" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="45" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="47">
         <v>2</v>
@@ -1195,10 +1207,10 @@
     </row>
     <row r="23" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="45" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="47">
         <v>2</v>
@@ -1210,7 +1222,7 @@
     </row>
     <row r="24" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="45" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B24" s="46" t="s">
         <v>13</v>
@@ -1225,7 +1237,7 @@
     </row>
     <row r="25" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="45" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B25" s="46" t="s">
         <v>13</v>
@@ -1240,7 +1252,7 @@
     </row>
     <row r="26" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="45" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B26" s="46" t="s">
         <v>13</v>
@@ -1252,6 +1264,60 @@
         <v>16</v>
       </c>
       <c r="E26" s="48"/>
+    </row>
+    <row r="27" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="47">
+        <v>2</v>
+      </c>
+      <c r="D27" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="48"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Minor updates. Continued level building
</commit_message>
<xml_diff>
--- a/Design Docs/Tasks.xlsx
+++ b/Design Docs/Tasks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepos\SpellCaster-FPS-Thing\Design Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{312AD015-C4B0-4EB1-918E-8F0872AD2050}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57715EEC-7970-4139-98D1-98A90C7A194B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="60">
   <si>
     <t>Task Name</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Black screen in CrossScenePersisted Object</t>
+  </si>
+  <si>
+    <t>Split UI to multiple canvases</t>
   </si>
 </sst>
 </file>
@@ -448,7 +451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -548,6 +551,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -828,22 +840,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.33203125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="55.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="99.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="99.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -860,7 +872,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
@@ -877,7 +889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="24" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>5</v>
       </c>
@@ -894,7 +906,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
         <v>9</v>
       </c>
@@ -911,7 +923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>14</v>
       </c>
@@ -928,7 +940,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>15</v>
       </c>
@@ -945,7 +957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="39" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>20</v>
       </c>
@@ -962,7 +974,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>29</v>
       </c>
@@ -979,7 +991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>21</v>
       </c>
@@ -996,7 +1008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="44" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" s="44" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="s">
         <v>24</v>
       </c>
@@ -1013,7 +1025,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>26</v>
       </c>
@@ -1030,7 +1042,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="34" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" s="34" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>33</v>
       </c>
@@ -1047,7 +1059,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>37</v>
       </c>
@@ -1062,7 +1074,7 @@
       </c>
       <c r="E13" s="33"/>
     </row>
-    <row r="14" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>38</v>
       </c>
@@ -1077,7 +1089,7 @@
       </c>
       <c r="E14" s="33"/>
     </row>
-    <row r="15" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>39</v>
       </c>
@@ -1092,7 +1104,7 @@
       </c>
       <c r="E15" s="33"/>
     </row>
-    <row r="16" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
         <v>40</v>
       </c>
@@ -1109,7 +1121,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>42</v>
       </c>
@@ -1126,7 +1138,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="50" t="s">
         <v>44</v>
       </c>
@@ -1141,7 +1153,7 @@
       </c>
       <c r="E18" s="53"/>
     </row>
-    <row r="19" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>45</v>
       </c>
@@ -1158,69 +1170,69 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="45" t="s">
+    <row r="20" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="47">
+      <c r="C20" s="57">
         <v>1</v>
       </c>
-      <c r="D20" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="48" t="s">
+      <c r="D20" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="58" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="45" t="s">
+    <row r="21" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="47">
-        <v>2</v>
-      </c>
-      <c r="D21" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="48"/>
-    </row>
-    <row r="22" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="45" t="s">
+      <c r="C21" s="57">
+        <v>2</v>
+      </c>
+      <c r="D21" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="58"/>
+    </row>
+    <row r="22" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="47">
-        <v>2</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="48"/>
-    </row>
-    <row r="23" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="45" t="s">
+      <c r="C22" s="57">
+        <v>2</v>
+      </c>
+      <c r="D22" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="58"/>
+    </row>
+    <row r="23" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="47">
-        <v>2</v>
-      </c>
-      <c r="D23" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="48"/>
-    </row>
-    <row r="24" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="57">
+        <v>2</v>
+      </c>
+      <c r="D23" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="58"/>
+    </row>
+    <row r="24" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="45" t="s">
         <v>49</v>
       </c>
@@ -1235,7 +1247,7 @@
       </c>
       <c r="E24" s="48"/>
     </row>
-    <row r="25" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="45" t="s">
         <v>50</v>
       </c>
@@ -1250,7 +1262,7 @@
       </c>
       <c r="E25" s="48"/>
     </row>
-    <row r="26" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="45" t="s">
         <v>51</v>
       </c>
@@ -1265,7 +1277,7 @@
       </c>
       <c r="E26" s="48"/>
     </row>
-    <row r="27" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="45" t="s">
         <v>55</v>
       </c>
@@ -1280,44 +1292,63 @@
       </c>
       <c r="E27" s="48"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="7" t="s">
+    <row r="28" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="47">
         <v>1</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="7" t="s">
+      <c r="D28" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="48"/>
+    </row>
+    <row r="29" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="7" t="s">
+      <c r="C29" s="47">
+        <v>2</v>
+      </c>
+      <c r="D29" s="47"/>
+      <c r="E29" s="48"/>
+    </row>
+    <row r="30" spans="1:5" s="59" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="55" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="57">
         <v>1</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="D30" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="58"/>
+    </row>
+    <row r="31" spans="1:5" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="47">
+        <v>2</v>
+      </c>
+      <c r="D31" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="48"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>